<commit_message>
adding bacterial go to go sum xls
</commit_message>
<xml_diff>
--- a/analyses/unipept/GO-terms/GO-summary.xlsx
+++ b/analyses/unipept/GO-terms/GO-summary.xlsx
@@ -5,14 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="322-trypsin" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="323-trypsin" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="324-trypsin" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="325-trypsin" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="PCA-input" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="329-undigested" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="330-undigested" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="331-undigested" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="332-undigested" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="PCA-input" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,9 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="122">
-  <si>
-    <t xml:space="preserve">322-DB DIATOM</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="142">
+  <si>
+    <t xml:space="preserve">DIATOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB</t>
   </si>
   <si>
     <t xml:space="preserve">Peptides</t>
@@ -215,15 +222,48 @@
     <t xml:space="preserve">DN80</t>
   </si>
   <si>
-    <t xml:space="preserve">DB</t>
+    <t xml:space="preserve">BACTERIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plasma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0008076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voltage-gated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">potassium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0030288</t>
+  </si>
+  <si>
+    <t xml:space="preserve">periplasmic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009279</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0005623</t>
   </si>
   <si>
-    <t xml:space="preserve">cell</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0022625</t>
   </si>
   <si>
@@ -251,9 +291,6 @@
     <t xml:space="preserve">chaperone</t>
   </si>
   <si>
-    <t xml:space="preserve">complex</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0005750</t>
   </si>
   <si>
@@ -272,12 +309,6 @@
     <t xml:space="preserve">mitochondrion</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005886</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plasma</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0009539</t>
   </si>
   <si>
@@ -288,6 +319,39 @@
   </si>
   <si>
     <t xml:space="preserve">plastid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009521</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0016471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vacuolar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proton-transporting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATPase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0000220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vacuolar proton-transporting V-type ATPase, V0 domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0033179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proton-transporting V-type ATPase, V0 domain</t>
   </si>
   <si>
     <t xml:space="preserve">cumulative</t>
@@ -490,10 +554,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -510,137 +574,124 @@
       <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(D3,E3,F3,G3,H3)</f>
-        <v>integralcomponentofmembrane</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D4,E4,F4,G4,H4)</f>
-        <v>chloroplastthylakoidmembrane</v>
+        <v>integralcomponentofmembrane</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="G4" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D5,E5,F5,G5,H5)</f>
-        <v>chloroplast</v>
+        <v>chloroplastthylakoidmembrane</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D6,E6,F6,G6,H6)</f>
-        <v>photosystemIreactioncenter</v>
+        <v>chloroplast</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D7,E7,F7,G7,H7)</f>
-        <v>cytosolicsmallribosomalsubunit</v>
+        <v>photosystemIreactioncenter</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D8,E8,F8,G8,H8)</f>
-        <v>photosystemI</v>
+        <v>cytosolicsmallribosomalsubunit</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -652,10 +703,13 @@
       </c>
       <c r="C9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D9,E9,F9,G9,H9)</f>
-        <v>cytoplasm</v>
+        <v>photosystemI</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>25</v>
+        <v>15</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,20 +717,14 @@
         <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D10,E10,F10,G10,H10)</f>
-        <v>smallribosomalsubunit</v>
+        <v>cytoplasm</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,10 +736,16 @@
       </c>
       <c r="C11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D11,E11,F11,G11,H11)</f>
-        <v>cytosol</v>
+        <v>smallribosomalsubunit</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -699,29 +753,29 @@
         <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D12,E12,F12,G12,H12)</f>
-        <v>membrane</v>
+        <v>cytosol</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D13,E13,F13,G13,H13)</f>
-        <v>ribosome</v>
+        <v>membrane</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -729,14 +783,14 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D14,E14,F14,G14,H14)</f>
-        <v>proton-transporting ATP synthase complex, catalytic core F(1)</v>
+        <v>ribosome</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,14 +798,14 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D15,E15,F15,G15,H15)</f>
-        <v>proton-transporting ATP synthase complex, coupling factor F(o)</v>
+        <v>proton-transporting ATP synthase complex, catalytic core F(1)</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,20 +813,14 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D16,E16,F16,G16,H16)</f>
-        <v>COPIvesiclecoat</v>
+        <v>proton-transporting ATP synthase complex, coupling factor F(o)</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -780,17 +828,20 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D17,E17,F17,G17,H17)</f>
-        <v>Golgiapparatus</v>
+        <v>COPIvesiclecoat</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,23 +849,17 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D18,E18,F18,G18,H18)</f>
-        <v>endoplasmicreticulum-Golgiintermediatecompartment</v>
+        <v>Golgiapparatus</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,17 +867,23 @@
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D19,E19,F19,G19,H19)</f>
-        <v>endoplasmicreticulum</v>
+        <v>endoplasmicreticulum-Golgiintermediatecompartment</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -840,17 +891,17 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D20,E20,F20,G20,H20)</f>
-        <v>Golgimembrane</v>
+        <v>endoplasmicreticulum</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,16 +913,13 @@
       </c>
       <c r="C21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D21,E21,F21,G21,H21)</f>
-        <v>intracellularmembrane-boundedorganelle</v>
+        <v>Golgimembrane</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,20 +927,20 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D22,E22,F22,G22,H22)</f>
-        <v>mitochondrialoutermembrane</v>
+        <v>intracellularmembrane-boundedorganelle</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -900,17 +948,20 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C23" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D23,E23,F23,G23,H23)</f>
-        <v>chloroplastthylakoid</v>
+        <v>mitochondrialoutermembrane</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>11</v>
+        <v>58</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,22 +973,13 @@
       </c>
       <c r="C24" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D24,E24,F24,G24,H24)</f>
-        <v>integralcomponentofthylakoidmembrane</v>
+        <v>chloroplastthylakoid</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -949,89 +991,311 @@
       </c>
       <c r="C25" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D25,E25,F25,G25,H25)</f>
+        <v>integralcomponentofthylakoidmembrane</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(D26,E26,F26,G26,H26)</f>
         <v>photosystemII</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="D26" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B28" s="0" t="s">
+      <c r="D28" s="0" t="s">
         <v>4</v>
-      </c>
-      <c r="C28" s="1" t="str">
-        <f aca="false">_xlfn.CONCAT(D28,E28,F28,G28,H28)</f>
-        <v>integralcomponentofmembrane</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>9</v>
       </c>
       <c r="C29" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D29,E29,F29,G29,H29)</f>
-        <v>chloroplastthylakoidmembrane</v>
+        <v>integralcomponentofmembrane</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="G29" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C30" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D30,E30,F30,G30,H30)</f>
+        <v>chloroplastthylakoidmembrane</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(D31,E31,F31,G31,H31)</f>
         <v>chloroplast</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>10</v>
+      <c r="D31" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1070,18 +1334,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,23 +1353,23 @@
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D3,E3,F3,G3,H3)</f>
         <v>integralcomponentofmembrane</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,20 +1377,20 @@
         <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D4,E4,F4,G4,H4)</f>
         <v>chloroplastthylakoidmembrane</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,14 +1398,14 @@
         <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D5,E5,F5,G5,H5)</f>
         <v>chloroplast</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1149,14 +1413,14 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D6,E6,F6,G6,H6)</f>
         <v>cytoplasm</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1164,14 +1428,14 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D7,E7,F7,G7,H7)</f>
         <v>cell</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,14 +1443,14 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D8,E8,F8,G8,H8)</f>
         <v>ribosome</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1194,23 +1458,23 @@
         <v>2</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D9,E9,F9,G9,H9)</f>
         <v>photosystemIreactioncenter</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1218,14 +1482,14 @@
         <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D10,E10,F10,G10,H10)</f>
         <v>cytosol</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,14 +1497,14 @@
         <v>2</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D11,E11,F11,G11,H11)</f>
         <v>proton-transporting ATP synthase complex, catalytic core F(1)</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1248,17 +1512,17 @@
         <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D12,E12,F12,G12,H12)</f>
         <v>photosystemII</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,20 +1530,20 @@
         <v>1</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D13,E13,F13,G13,H13)</f>
         <v>smallribosomalsubunit</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,23 +1551,23 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D14,E14,F14,G14,H14)</f>
         <v>cytosolicsmallribosomalsubunit</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1311,23 +1575,23 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C15" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D15,E15,F15,G15,H15)</f>
         <v>cytosoliclargeribosomalsubunit</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1335,23 +1599,23 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C16" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D16,E16,F16,G16,H16)</f>
         <v>mitochondriallargeribosomalsubunit</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1359,14 +1623,14 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D17,E17,F17,G17,H17)</f>
         <v>membrane</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1374,20 +1638,20 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C18" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D18,E18,F18,G18,H18)</f>
         <v>endoplasmicreticulumlumen</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1395,14 +1659,14 @@
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C19" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D19,E19,F19,G19,H19)</f>
         <v>nucleus</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1410,23 +1674,23 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C20" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D20,E20,F20,G20,H20)</f>
         <v>endoplasmicreticulumchaperonecomplex</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1434,26 +1698,26 @@
         <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C21" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D21,E21,F21,G21,H21)</f>
         <v>mitochondrialrespiratorychaincomplexIII</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1461,14 +1725,14 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C22" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D22,E22,F22,G22,H22)</f>
         <v>mitochondrion</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1476,33 +1740,33 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C23" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D23,E23,F23,G23,H23)</f>
         <v>plasmamembrane</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1510,14 +1774,14 @@
         <v>4</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D26,E26,F26,G26,H26)</f>
         <v>cytoplasm</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1525,23 +1789,23 @@
         <v>4</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C27" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D27,E27,F27,G27,H27)</f>
         <v>integralcomponentofmembrane</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1549,14 +1813,14 @@
         <v>3</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C28" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D28,E28,F28,G28,H28)</f>
         <v>chloroplast</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1564,20 +1828,20 @@
         <v>2</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C29" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D29,E29,F29,G29,H29)</f>
         <v>chloroplastthylakoidmembrane</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1585,23 +1849,23 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C30" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D30,E30,F30,G30,H30)</f>
         <v>photosystemIreactioncenter</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1609,14 +1873,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D31,E31,F31,G31,H31)</f>
         <v>membrane</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1624,20 +1888,20 @@
         <v>1</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C32" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D32,E32,F32,G32,H32)</f>
         <v>endoplasmicreticulumlumen</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1645,14 +1909,14 @@
         <v>1</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C33" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D33,E33,F33,G33,H33)</f>
         <v>nucleus</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1660,23 +1924,23 @@
         <v>1</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C34" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D34,E34,F34,G34,H34)</f>
         <v>endoplasmicreticulumchaperonecomplex</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1684,17 +1948,17 @@
         <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C35" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D35,E35,F35,G35,H35)</f>
         <v>photosystemII</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1726,18 +1990,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,23 +2009,23 @@
         <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D3,E3,F3,G3,H3)</f>
         <v>integralcomponentofmembrane</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1769,20 +2033,20 @@
         <v>20</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D4,E4,F4,G4,H4)</f>
         <v>chloroplastthylakoidmembrane</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,14 +2054,14 @@
         <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D5,E5,F5,G5,H5)</f>
         <v>chloroplast</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,23 +2069,23 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D6,E6,F6,G6,H6)</f>
         <v>photosystemIreactioncenter</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1829,26 +2093,26 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D7,E7,F7,G7,H7)</f>
         <v>integralcomponentofthylakoidmembrane</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1856,14 +2120,14 @@
         <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D8,E8,F8,G8,H8)</f>
         <v>cytoplasm</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1871,17 +2135,17 @@
         <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D9,E9,F9,G9,H9)</f>
         <v>photosystemI</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1889,39 +2153,39 @@
         <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D10,E10,F10,G10,H10)</f>
         <v>photosystemIIreactioncenter</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,23 +2193,23 @@
         <v>6</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D13,E13,F13,G13,H13)</f>
         <v>integralcomponentofmembrane</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,14 +2217,14 @@
         <v>3</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D14,E14,F14,G14,H14)</f>
         <v>chloroplast</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1968,20 +2232,20 @@
         <v>3</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D15,E15,F15,G15,H15)</f>
         <v>chloroplastthylakoidmembrane</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,23 +2253,23 @@
         <v>2</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D16,E16,F16,G16,H16)</f>
         <v>photosystemIreactioncenter</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2041,18 +2305,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2060,23 +2324,23 @@
         <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D3,E3,F3,G3,H3)</f>
         <v>integralcomponentofmembrane</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2084,20 +2348,20 @@
         <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D4,E4,F4,G4,H4)</f>
         <v>chloroplastthylakoidmembrane</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2105,14 +2369,14 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D5,E5,F5,G5,H5)</f>
         <v>chloroplast</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2120,23 +2384,23 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D6,E6,F6,G6,H6)</f>
         <v>photosystemIreactioncenter</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2144,39 +2408,39 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D7,E7,F7,G7,H7)</f>
         <v>photosystemIIreactioncenter</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2184,23 +2448,23 @@
         <v>7</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D10,E10,F10,G10,H10)</f>
         <v>integralcomponentofmembrane</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2208,20 +2472,20 @@
         <v>6</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D11,E11,F11,G11,H11)</f>
         <v>chloroplastthylakoidmembrane</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2229,14 +2493,14 @@
         <v>3</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D12,E12,F12,G12,H12)</f>
         <v>chloroplast</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2244,23 +2508,23 @@
         <v>1</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D13,E13,F13,G13,H13)</f>
         <v>photosystemIreactioncenter</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2268,17 +2532,17 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D14,E14,F14,G14,H14)</f>
         <v>photosystemI</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2286,14 +2550,14 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C15" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(D15,E15,F15,G15,H15)</f>
         <v>plastid</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2312,10 +2576,494 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2325,7 +3073,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>322</v>
@@ -2340,15 +3088,15 @@
         <v>325</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>39</v>
@@ -2367,12 +3115,12 @@
         <v>92</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>30</v>
@@ -2391,12 +3139,12 @@
         <v>76</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>14</v>
@@ -2415,12 +3163,12 @@
         <v>34</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
@@ -2439,12 +3187,12 @@
         <v>17</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2</v>
@@ -2460,12 +3208,12 @@
         <v>14</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>13</v>
@@ -2475,7 +3223,7 @@
         <v>13</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="J7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(K7,L7,M7,N7,O7)</f>
@@ -2484,7 +3232,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
@@ -2500,12 +3248,12 @@
         <v>6</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>5</v>
@@ -2515,12 +3263,12 @@
         <v>5</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>4</v>
@@ -2533,12 +3281,12 @@
         <v>5</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2</v>
@@ -2551,12 +3299,12 @@
         <v>4</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
@@ -2569,12 +3317,12 @@
         <v>4</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>2</v>
@@ -2590,12 +3338,12 @@
         <v>4</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>2</v>
@@ -2608,12 +3356,12 @@
         <v>4</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>2</v>
@@ -2626,12 +3374,12 @@
         <v>3</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>2</v>
@@ -2641,12 +3389,12 @@
         <v>2</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
@@ -2659,12 +3407,12 @@
         <v>2</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>1</v>
@@ -2677,12 +3425,12 @@
         <v>2</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
@@ -2692,12 +3440,12 @@
         <v>1</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1</v>
@@ -2707,12 +3455,12 @@
         <v>1</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
@@ -2722,12 +3470,12 @@
         <v>1</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1</v>
@@ -2737,12 +3485,12 @@
         <v>1</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>1</v>
@@ -2752,12 +3500,12 @@
         <v>1</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1</v>
@@ -2767,12 +3515,12 @@
         <v>1</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>1</v>
@@ -2782,12 +3530,12 @@
         <v>1</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1</v>
@@ -2797,12 +3545,12 @@
         <v>1</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>1</v>
@@ -2812,12 +3560,12 @@
         <v>1</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1</v>
@@ -2827,12 +3575,12 @@
         <v>1</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>1</v>
@@ -2842,12 +3590,12 @@
         <v>1</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -2857,12 +3605,12 @@
         <v>1</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
@@ -2872,12 +3620,12 @@
         <v>1</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -2887,12 +3635,12 @@
         <v>1</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
@@ -2902,12 +3650,12 @@
         <v>1</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>1</v>
@@ -2915,7 +3663,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
finished bacterial cc go in summary xls
</commit_message>
<xml_diff>
--- a/analyses/unipept/GO-terms/GO-summary.xlsx
+++ b/analyses/unipept/GO-terms/GO-summary.xlsx
@@ -21,14 +21,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="186">
   <si>
     <t xml:space="preserve">DIATOM</t>
   </si>
@@ -495,46 +495,73 @@
     <t xml:space="preserve">GO:0016021 integral component of membrane</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0009538 photosystem I reaction center</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0009535 chloroplast thylakoid membrane</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0009507 chloroplast</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0009538 photosystem I reaction center</t>
+    <t xml:space="preserve">GO:0005886 plasma membrane </t>
   </si>
   <si>
     <t xml:space="preserve">GO:0005737 cytoplasm</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0045263 proton-transporting ATP synthase complex, coupling factor F(o)</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0005634 nucleus</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0043231 intracellular membrane-bounded organelle</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0045261 proton-transporting ATP synthase complex, catalytic core F(1)</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0005794 Golgi apparatus</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0005623 cell </t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0005793 endoplasmic reticulum-Golgi intermediate compartment</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0022627 cytosolic small ribosomal subunit</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0005783 endoplasmic reticulum</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0005829 cytosol</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0005739 mitochondrion </t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0005840 ribosome</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0009522 photosystem I</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0015935 small ribosomal subunit</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0016020 membrane</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0015935 small ribosomal subunit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005788 endoplasmic reticulumlumen</t>
+    <t xml:space="preserve">GO:0009536 plastid </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0030126 COPI vesicle coat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005788 endoplasmic reticulum lumen</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0009523 photosystem II</t>
@@ -546,9 +573,6 @@
     <t xml:space="preserve">GO:0000139 Golgi membrane</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005739 mitochondrion </t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0005741 mitochondrial outer membrane</t>
   </si>
   <si>
@@ -558,43 +582,18 @@
     <t xml:space="preserve">GO:0005762 mitochondrial large ribosomal subunit </t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005783 endoplasmic reticulum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005793 endoplasmic reticulum-Golgi intermediate compartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005794 Golgi apparatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005886 plasma membrane </t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0009534 chloroplast thylakoid</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0009536 plastid </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0030126 COPI vesicle coat</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0031361 integral component of thylakoid membrane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0043231 intracellular membrane-bounded organelle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0045263 proton-transporting ATP synthase complex, coupling factor F(o)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -618,12 +617,72 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDE59"/>
+        <bgColor rgb="FFD4EA6B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD4EA6B"/>
+        <bgColor rgb="FFFFDE59"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FFB4C7DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA6A6"/>
+        <bgColor rgb="FFFFD8CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7B59"/>
+        <bgColor rgb="FFFF5429"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEE6EF"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD8CE"/>
+        <bgColor rgb="FFDEE6EF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8A202"/>
+        <bgColor rgb="FFFF7B59"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5429"/>
+        <bgColor rgb="FFFF7B59"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -660,12 +719,56 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -678,6 +781,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB4C7DC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFDEE6EF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF7B59"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFD4EA6B"/>
+      <rgbColor rgb="FFAFD095"/>
+      <rgbColor rgb="FFFFA6A6"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFD8CE"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFDE59"/>
+      <rgbColor rgb="FFE8A202"/>
+      <rgbColor rgb="FFFF5429"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1182,7 +1345,7 @@
       <c r="B29" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="1" t="str">
+      <c r="C29" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D29,E29,F29,G29,H29)</f>
         <v>integralcomponentofmembrane</v>
       </c>
@@ -1206,7 +1369,7 @@
       <c r="B30" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="1" t="str">
+      <c r="C30" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D30,E30,F30,G30,H30)</f>
         <v>chloroplastthylakoidmembrane</v>
       </c>
@@ -1227,7 +1390,7 @@
       <c r="B31" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="1" t="str">
+      <c r="C31" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D31,E31,F31,G31,H31)</f>
         <v>chloroplast</v>
       </c>
@@ -1432,11 +1595,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1492,7 +1655,7 @@
       <c r="B4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="str">
+      <c r="C4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D4,E4,F4,G4,H4)</f>
         <v>integralcomponentofmembrane</v>
       </c>
@@ -1516,7 +1679,7 @@
       <c r="B5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="str">
+      <c r="C5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D5,E5,F5,G5,H5)</f>
         <v>chloroplastthylakoidmembrane</v>
       </c>
@@ -1537,7 +1700,7 @@
       <c r="B6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="str">
+      <c r="C6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D6,E6,F6,G6,H6)</f>
         <v>chloroplast</v>
       </c>
@@ -1552,7 +1715,7 @@
       <c r="B7" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="str">
+      <c r="C7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D7,E7,F7,G7,H7)</f>
         <v>cytoplasm</v>
       </c>
@@ -1567,7 +1730,7 @@
       <c r="B8" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="1" t="str">
+      <c r="C8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D8,E8,F8,G8,H8)</f>
         <v>cell</v>
       </c>
@@ -1582,7 +1745,7 @@
       <c r="B9" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="1" t="str">
+      <c r="C9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D9,E9,F9,G9,H9)</f>
         <v>ribosome</v>
       </c>
@@ -1597,7 +1760,7 @@
       <c r="B10" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1" t="str">
+      <c r="C10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D10,E10,F10,G10,H10)</f>
         <v>photosystemIreactioncenter</v>
       </c>
@@ -1621,7 +1784,7 @@
       <c r="B11" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="1" t="str">
+      <c r="C11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D11,E11,F11,G11,H11)</f>
         <v>cytosol</v>
       </c>
@@ -1636,7 +1799,7 @@
       <c r="B12" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1" t="str">
+      <c r="C12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D12,E12,F12,G12,H12)</f>
         <v>proton-transporting ATP synthase complex, catalytic core F(1)</v>
       </c>
@@ -1651,7 +1814,7 @@
       <c r="B13" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="1" t="str">
+      <c r="C13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D13,E13,F13,G13,H13)</f>
         <v>photosystemII</v>
       </c>
@@ -1669,7 +1832,7 @@
       <c r="B14" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="1" t="str">
+      <c r="C14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D14,E14,F14,G14,H14)</f>
         <v>smallribosomalsubunit</v>
       </c>
@@ -1690,7 +1853,7 @@
       <c r="B15" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="1" t="str">
+      <c r="C15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D15,E15,F15,G15,H15)</f>
         <v>cytosolicsmallribosomalsubunit</v>
       </c>
@@ -1714,7 +1877,7 @@
       <c r="B16" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="1" t="str">
+      <c r="C16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D16,E16,F16,G16,H16)</f>
         <v>cytosoliclargeribosomalsubunit</v>
       </c>
@@ -1738,7 +1901,7 @@
       <c r="B17" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="1" t="str">
+      <c r="C17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D17,E17,F17,G17,H17)</f>
         <v>mitochondriallargeribosomalsubunit</v>
       </c>
@@ -1762,7 +1925,7 @@
       <c r="B18" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="1" t="str">
+      <c r="C18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D18,E18,F18,G18,H18)</f>
         <v>membrane</v>
       </c>
@@ -1777,7 +1940,7 @@
       <c r="B19" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="1" t="str">
+      <c r="C19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D19,E19,F19,G19,H19)</f>
         <v>endoplasmicreticulumlumen</v>
       </c>
@@ -1798,7 +1961,7 @@
       <c r="B20" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="1" t="str">
+      <c r="C20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D20,E20,F20,G20,H20)</f>
         <v>nucleus</v>
       </c>
@@ -1813,7 +1976,7 @@
       <c r="B21" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="1" t="str">
+      <c r="C21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D21,E21,F21,G21,H21)</f>
         <v>endoplasmicreticulumchaperonecomplex</v>
       </c>
@@ -1837,7 +2000,7 @@
       <c r="B22" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="1" t="str">
+      <c r="C22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D22,E22,F22,G22,H22)</f>
         <v>mitochondrialrespiratorychaincomplexIII</v>
       </c>
@@ -1864,7 +2027,7 @@
       <c r="B23" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="1" t="str">
+      <c r="C23" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D23,E23,F23,G23,H23)</f>
         <v>mitochondrion</v>
       </c>
@@ -1879,7 +2042,7 @@
       <c r="B24" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="1" t="str">
+      <c r="C24" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D24,E24,F24,G24,H24)</f>
         <v>plasmamembrane</v>
       </c>
@@ -1913,7 +2076,7 @@
       <c r="B27" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="1" t="str">
+      <c r="C27" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D27,E27,F27,G27,H27)</f>
         <v>cytoplasm</v>
       </c>
@@ -1928,7 +2091,7 @@
       <c r="B28" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="1" t="str">
+      <c r="C28" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D28,E28,F28,G28,H28)</f>
         <v>integralcomponentofmembrane</v>
       </c>
@@ -1952,7 +2115,7 @@
       <c r="B29" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="1" t="str">
+      <c r="C29" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D29,E29,F29,G29,H29)</f>
         <v>chloroplast</v>
       </c>
@@ -1967,7 +2130,7 @@
       <c r="B30" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="1" t="str">
+      <c r="C30" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D30,E30,F30,G30,H30)</f>
         <v>chloroplastthylakoidmembrane</v>
       </c>
@@ -1988,7 +2151,7 @@
       <c r="B31" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="1" t="str">
+      <c r="C31" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D31,E31,F31,G31,H31)</f>
         <v>photosystemIreactioncenter</v>
       </c>
@@ -2012,7 +2175,7 @@
       <c r="B32" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="1" t="str">
+      <c r="C32" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D32,E32,F32,G32,H32)</f>
         <v>membrane</v>
       </c>
@@ -2027,7 +2190,7 @@
       <c r="B33" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="1" t="str">
+      <c r="C33" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D33,E33,F33,G33,H33)</f>
         <v>endoplasmicreticulumlumen</v>
       </c>
@@ -2048,7 +2211,7 @@
       <c r="B34" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="1" t="str">
+      <c r="C34" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D34,E34,F34,G34,H34)</f>
         <v>nucleus</v>
       </c>
@@ -2063,7 +2226,7 @@
       <c r="B35" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="1" t="str">
+      <c r="C35" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D35,E35,F35,G35,H35)</f>
         <v>endoplasmicreticulumchaperonecomplex</v>
       </c>
@@ -2087,7 +2250,7 @@
       <c r="B36" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="1" t="str">
+      <c r="C36" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D36,E36,F36,G36,H36)</f>
         <v>photosystemII</v>
       </c>
@@ -2286,11 +2449,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2339,7 +2502,7 @@
       <c r="B4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="str">
+      <c r="C4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D4,E4,F4,G4,H4)</f>
         <v>integralcomponentofmembrane</v>
       </c>
@@ -2363,7 +2526,7 @@
       <c r="B5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="str">
+      <c r="C5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D5,E5,F5,G5,H5)</f>
         <v>chloroplastthylakoidmembrane</v>
       </c>
@@ -2384,7 +2547,7 @@
       <c r="B6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="str">
+      <c r="C6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D6,E6,F6,G6,H6)</f>
         <v>chloroplast</v>
       </c>
@@ -2399,7 +2562,7 @@
       <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="str">
+      <c r="C7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D7,E7,F7,G7,H7)</f>
         <v>photosystemIreactioncenter</v>
       </c>
@@ -2423,7 +2586,7 @@
       <c r="B8" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="1" t="str">
+      <c r="C8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D8,E8,F8,G8,H8)</f>
         <v>integralcomponentofthylakoidmembrane</v>
       </c>
@@ -2450,7 +2613,7 @@
       <c r="B9" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="1" t="str">
+      <c r="C9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D9,E9,F9,G9,H9)</f>
         <v>cytoplasm</v>
       </c>
@@ -2465,7 +2628,7 @@
       <c r="B10" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="1" t="str">
+      <c r="C10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D10,E10,F10,G10,H10)</f>
         <v>photosystemI</v>
       </c>
@@ -2483,7 +2646,7 @@
       <c r="B11" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="C11" s="1" t="str">
+      <c r="C11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D11,E11,F11,G11,H11)</f>
         <v>photosystemIIreactioncenter</v>
       </c>
@@ -2523,7 +2686,7 @@
       <c r="B14" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="1" t="str">
+      <c r="C14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D14,E14,F14,G14,H14)</f>
         <v>integralcomponentofmembrane</v>
       </c>
@@ -2547,7 +2710,7 @@
       <c r="B15" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1" t="str">
+      <c r="C15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D15,E15,F15,G15,H15)</f>
         <v>chloroplast</v>
       </c>
@@ -2562,7 +2725,7 @@
       <c r="B16" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="1" t="str">
+      <c r="C16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D16,E16,F16,G16,H16)</f>
         <v>chloroplastthylakoidmembrane</v>
       </c>
@@ -2583,7 +2746,7 @@
       <c r="B17" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="1" t="str">
+      <c r="C17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D17,E17,F17,G17,H17)</f>
         <v>photosystemIreactioncenter</v>
       </c>
@@ -2788,11 +2951,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2845,7 +3008,7 @@
       <c r="B4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="str">
+      <c r="C4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D4,E4,F4,G4,H4)</f>
         <v>integralcomponentofmembrane</v>
       </c>
@@ -2869,7 +3032,7 @@
       <c r="B5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="str">
+      <c r="C5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D5,E5,F5,G5,H5)</f>
         <v>chloroplastthylakoidmembrane</v>
       </c>
@@ -2890,7 +3053,7 @@
       <c r="B6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="str">
+      <c r="C6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D6,E6,F6,G6,H6)</f>
         <v>chloroplast</v>
       </c>
@@ -2905,7 +3068,7 @@
       <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="str">
+      <c r="C7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D7,E7,F7,G7,H7)</f>
         <v>photosystemIreactioncenter</v>
       </c>
@@ -2929,7 +3092,7 @@
       <c r="B8" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="1" t="str">
+      <c r="C8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D8,E8,F8,G8,H8)</f>
         <v>photosystemIIreactioncenter</v>
       </c>
@@ -2969,7 +3132,7 @@
       <c r="B11" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1" t="str">
+      <c r="C11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D11,E11,F11,G11,H11)</f>
         <v>integralcomponentofmembrane</v>
       </c>
@@ -2993,7 +3156,7 @@
       <c r="B12" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1" t="str">
+      <c r="C12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D12,E12,F12,G12,H12)</f>
         <v>chloroplastthylakoidmembrane</v>
       </c>
@@ -3014,7 +3177,7 @@
       <c r="B13" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="1" t="str">
+      <c r="C13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D13,E13,F13,G13,H13)</f>
         <v>chloroplast</v>
       </c>
@@ -3029,7 +3192,7 @@
       <c r="B14" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="1" t="str">
+      <c r="C14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D14,E14,F14,G14,H14)</f>
         <v>photosystemIreactioncenter</v>
       </c>
@@ -3053,7 +3216,7 @@
       <c r="B15" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="1" t="str">
+      <c r="C15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D15,E15,F15,G15,H15)</f>
         <v>photosystemI</v>
       </c>
@@ -3071,7 +3234,7 @@
       <c r="B16" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="1" t="str">
+      <c r="C16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D16,E16,F16,G16,H16)</f>
         <v>plastid</v>
       </c>
@@ -3250,11 +3413,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3653,11 +3816,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4481,11 +4644,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4684,11 +4847,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4912,11 +5075,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4926,15 +5089,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P29" activeCellId="0" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="42.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="55.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4976,6 +5140,21 @@
       <c r="M2" s="0" t="s">
         <v>153</v>
       </c>
+      <c r="O2" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -4997,7 +5176,7 @@
         <f aca="false">SUM(B3:E3)</f>
         <v>92</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>154</v>
       </c>
       <c r="J3" s="0" t="n">
@@ -5011,6 +5190,25 @@
       </c>
       <c r="M3" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <f aca="false">J6+J14+J18+J19</f>
+        <v>8</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <f aca="false">K6+K14+K18+K19</f>
+        <v>2</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <f aca="false">L6+L14+L18+L19</f>
+        <v>8</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <f aca="false">M6+M14+M18+M19</f>
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5033,8 +5231,8 @@
         <f aca="false">SUM(B4:E4)</f>
         <v>76</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>155</v>
+      <c r="I4" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>30</v>
@@ -5047,6 +5245,25 @@
       </c>
       <c r="M4" s="0" t="n">
         <v>22</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <f aca="false">J4+J5+J29+J32</f>
+        <v>46</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <f aca="false">K4+K5+K29+K32</f>
+        <v>2</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <f aca="false">L4+L5+L29+L32</f>
+        <v>34</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <f aca="false">M4+M5+M29+M32</f>
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5069,8 +5286,8 @@
         <f aca="false">SUM(B5:E5)</f>
         <v>34</v>
       </c>
-      <c r="I5" s="0" t="s">
-        <v>156</v>
+      <c r="I5" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>14</v>
@@ -5083,6 +5300,25 @@
       </c>
       <c r="M5" s="0" t="n">
         <v>8</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <f aca="false">J3+J15</f>
+        <v>41</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <f aca="false">K3+K15</f>
+        <v>3</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <f aca="false">L3+L15</f>
+        <v>28</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <f aca="false">M3+M15</f>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5105,8 +5341,8 @@
         <f aca="false">SUM(B6:E6)</f>
         <v>17</v>
       </c>
-      <c r="I6" s="0" t="s">
-        <v>157</v>
+      <c r="I6" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>5</v>
@@ -5119,6 +5355,21 @@
       </c>
       <c r="M6" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5138,8 +5389,8 @@
         <f aca="false">SUM(B7:E7)</f>
         <v>14</v>
       </c>
-      <c r="I7" s="0" t="s">
-        <v>158</v>
+      <c r="I7" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>2</v>
@@ -5151,6 +5402,25 @@
         <v>2</v>
       </c>
       <c r="M7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <f aca="false">J34+J9</f>
+        <v>2</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <f aca="false">K34+K9</f>
+        <v>2</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <f aca="false">L34+L9</f>
+        <v>3</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <f aca="false">M34+M9</f>
         <v>0</v>
       </c>
     </row>
@@ -5165,8 +5435,8 @@
         <f aca="false">SUM(B8:E8)</f>
         <v>13</v>
       </c>
-      <c r="I8" s="0" t="s">
-        <v>159</v>
+      <c r="I8" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -5178,6 +5448,25 @@
         <v>0</v>
       </c>
       <c r="M8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <f aca="false">J33+J8</f>
+        <v>1</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <f aca="false">K33+K8</f>
+        <v>13</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <f aca="false">L33+L8</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <f aca="false">M33+M8</f>
         <v>0</v>
       </c>
     </row>
@@ -5198,8 +5487,8 @@
         <f aca="false">SUM(B9:E9)</f>
         <v>6</v>
       </c>
-      <c r="I9" s="0" t="s">
-        <v>160</v>
+      <c r="I9" s="7" t="s">
+        <v>163</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>1</v>
@@ -5211,6 +5500,25 @@
         <v>3</v>
       </c>
       <c r="M9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <f aca="false">J20+J27</f>
+        <v>2</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <f aca="false">K20+K27</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <f aca="false">L20+L27</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <f aca="false">M20+M27</f>
         <v>0</v>
       </c>
     </row>
@@ -5225,8 +5533,8 @@
         <f aca="false">SUM(B10:E10)</f>
         <v>5</v>
       </c>
-      <c r="I10" s="0" t="s">
-        <v>161</v>
+      <c r="I10" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -5238,6 +5546,21 @@
         <v>0</v>
       </c>
       <c r="M10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5255,8 +5578,8 @@
         <f aca="false">SUM(B11:E11)</f>
         <v>5</v>
       </c>
-      <c r="I11" s="0" t="s">
-        <v>162</v>
+      <c r="I11" s="8" t="s">
+        <v>167</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>4</v>
@@ -5268,6 +5591,25 @@
         <v>0</v>
       </c>
       <c r="M11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <f aca="false">J17+J25</f>
+        <v>1</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <f aca="false">K17+K25</f>
+        <v>2</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <f aca="false">L17+L25</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <f aca="false">M17+M25</f>
         <v>0</v>
       </c>
     </row>
@@ -5285,8 +5627,8 @@
         <f aca="false">SUM(B12:E12)</f>
         <v>4</v>
       </c>
-      <c r="I12" s="0" t="s">
-        <v>163</v>
+      <c r="I12" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>2</v>
@@ -5298,6 +5640,25 @@
         <v>0</v>
       </c>
       <c r="M12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <f aca="false">J21+J22+J23+J24</f>
+        <v>1</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <f aca="false">K21+K22+K23+K24</f>
+        <v>3</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <f aca="false">L21+L22+L23+L24</f>
+        <v>0</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <f aca="false">M21+M22+M23+M24</f>
         <v>0</v>
       </c>
     </row>
@@ -5316,7 +5677,7 @@
         <v>4</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>1</v>
@@ -5328,6 +5689,21 @@
         <v>0</v>
       </c>
       <c r="M13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5348,8 +5724,8 @@
         <f aca="false">SUM(B14:E14)</f>
         <v>4</v>
       </c>
-      <c r="I14" s="0" t="s">
-        <v>165</v>
+      <c r="I14" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>2</v>
@@ -5362,6 +5738,25 @@
       </c>
       <c r="M14" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <f aca="false">J16+J11</f>
+        <v>6</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <f aca="false">K16+K11</f>
+        <v>2</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <f aca="false">L16+L11</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <f aca="false">M16+M11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5378,8 +5773,8 @@
         <f aca="false">SUM(B15:E15)</f>
         <v>4</v>
       </c>
-      <c r="I15" s="0" t="s">
-        <v>166</v>
+      <c r="I15" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>2</v>
@@ -5392,6 +5787,21 @@
       </c>
       <c r="M15" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5408,8 +5818,8 @@
         <f aca="false">SUM(B16:E16)</f>
         <v>3</v>
       </c>
-      <c r="I16" s="0" t="s">
-        <v>167</v>
+      <c r="I16" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>2</v>
@@ -5421,6 +5831,21 @@
         <v>0</v>
       </c>
       <c r="M16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5435,8 +5860,8 @@
         <f aca="false">SUM(B17:E17)</f>
         <v>2</v>
       </c>
-      <c r="I17" s="0" t="s">
-        <v>168</v>
+      <c r="I17" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>0</v>
@@ -5448,6 +5873,25 @@
         <v>0</v>
       </c>
       <c r="M17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <f aca="false">J10+J12+J7</f>
+        <v>4</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <f aca="false">K10+K12+K7</f>
+        <v>17</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <f aca="false">L10+L12+L7</f>
+        <v>2</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <f aca="false">M10+M12+M7</f>
         <v>0</v>
       </c>
     </row>
@@ -5465,8 +5909,8 @@
         <f aca="false">SUM(B18:E18)</f>
         <v>2</v>
       </c>
-      <c r="I18" s="0" t="s">
-        <v>169</v>
+      <c r="I18" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>1</v>
@@ -5495,8 +5939,8 @@
         <f aca="false">SUM(B19:E19)</f>
         <v>2</v>
       </c>
-      <c r="I19" s="0" t="s">
-        <v>170</v>
+      <c r="I19" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>0</v>
@@ -5522,8 +5966,8 @@
         <f aca="false">SUM(B20:E20)</f>
         <v>1</v>
       </c>
-      <c r="I20" s="0" t="s">
-        <v>171</v>
+      <c r="I20" s="10" t="s">
+        <v>180</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>1</v>
@@ -5549,8 +5993,8 @@
         <f aca="false">SUM(B21:E21)</f>
         <v>1</v>
       </c>
-      <c r="I21" s="0" t="s">
-        <v>172</v>
+      <c r="I21" s="11" t="s">
+        <v>170</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>0</v>
@@ -5576,8 +6020,8 @@
         <f aca="false">SUM(B22:E22)</f>
         <v>1</v>
       </c>
-      <c r="I22" s="0" t="s">
-        <v>173</v>
+      <c r="I22" s="11" t="s">
+        <v>181</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>1</v>
@@ -5603,8 +6047,8 @@
         <f aca="false">SUM(B23:E23)</f>
         <v>1</v>
       </c>
-      <c r="I23" s="0" t="s">
-        <v>174</v>
+      <c r="I23" s="11" t="s">
+        <v>182</v>
       </c>
       <c r="J23" s="0" t="n">
         <v>0</v>
@@ -5630,8 +6074,8 @@
         <f aca="false">SUM(B24:E24)</f>
         <v>1</v>
       </c>
-      <c r="I24" s="0" t="s">
-        <v>175</v>
+      <c r="I24" s="11" t="s">
+        <v>183</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>0</v>
@@ -5657,8 +6101,8 @@
         <f aca="false">SUM(B25:E25)</f>
         <v>1</v>
       </c>
-      <c r="I25" s="0" t="s">
-        <v>176</v>
+      <c r="I25" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>1</v>
@@ -5684,8 +6128,8 @@
         <f aca="false">SUM(B26:E26)</f>
         <v>1</v>
       </c>
-      <c r="I26" s="0" t="s">
-        <v>177</v>
+      <c r="I26" s="12" t="s">
+        <v>166</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>1</v>
@@ -5711,8 +6155,8 @@
         <f aca="false">SUM(B27:E27)</f>
         <v>1</v>
       </c>
-      <c r="I27" s="0" t="s">
-        <v>178</v>
+      <c r="I27" s="10" t="s">
+        <v>164</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>1</v>
@@ -5739,7 +6183,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="J28" s="0" t="n">
         <v>0</v>
@@ -5765,8 +6209,8 @@
         <f aca="false">SUM(B29:E29)</f>
         <v>1</v>
       </c>
-      <c r="I29" s="0" t="s">
-        <v>180</v>
+      <c r="I29" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>1</v>
@@ -5793,7 +6237,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>0</v>
@@ -5820,7 +6264,7 @@
         <v>1</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="J31" s="0" t="n">
         <v>1</v>
@@ -5846,8 +6290,8 @@
         <f aca="false">SUM(B32:E32)</f>
         <v>1</v>
       </c>
-      <c r="I32" s="0" t="s">
-        <v>183</v>
+      <c r="I32" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="J32" s="0" t="n">
         <v>1</v>
@@ -5873,8 +6317,8 @@
         <f aca="false">SUM(B33:E33)</f>
         <v>1</v>
       </c>
-      <c r="I33" s="0" t="s">
-        <v>184</v>
+      <c r="I33" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>1</v>
@@ -5900,8 +6344,8 @@
         <f aca="false">SUM(B34:E34)</f>
         <v>1</v>
       </c>
-      <c r="I34" s="0" t="s">
-        <v>185</v>
+      <c r="I34" s="7" t="s">
+        <v>160</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>1</v>
@@ -5934,11 +6378,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
plotted GO terms in jupyter
</commit_message>
<xml_diff>
--- a/analyses/unipept/GO-terms/GO-summary.xlsx
+++ b/analyses/unipept/GO-terms/GO-summary.xlsx
@@ -16,7 +16,8 @@
     <sheet name="330-undigested" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="331-undigested" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="332-undigested" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="PCA-input" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="PCA-input-DIATOM" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="PCA-input-BACTERIA" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="194">
   <si>
     <t xml:space="preserve">DIATOM</t>
   </si>
@@ -309,9 +310,33 @@
     <t xml:space="preserve">mitochondrion</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0016021 integral component of membrane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005737 cytoplasm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005886 plasma membrane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0008076 voltage-gated potassium channel complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0030288 outer membrane-bounded periplasmic space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009279 cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0016020 membrane</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0009539</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0045261 proton-transporting ATP synthase complex, catalytic core F(1)</t>
+  </si>
+  <si>
     <t xml:space="preserve">325-DB</t>
   </si>
   <si>
@@ -321,6 +346,9 @@
     <t xml:space="preserve">plastid</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0009279 cell outer membrane</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0042597</t>
   </si>
   <si>
@@ -474,6 +502,9 @@
     <t xml:space="preserve">particle</t>
   </si>
   <si>
+    <t xml:space="preserve">Membrane:cytosol</t>
+  </si>
+  <si>
     <t xml:space="preserve">cumulative</t>
   </si>
   <si>
@@ -492,72 +523,63 @@
     <t xml:space="preserve">T12-325</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0016021 integral component of membrane</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0009538 photosystem I reaction center</t>
   </si>
   <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0009535 chloroplast thylakoid membrane</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0009507 chloroplast</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0009536 plastid </t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0005886 plasma membrane </t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005737 cytoplasm</t>
+    <t xml:space="preserve">GO:0005634 nucleus</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0045263 proton-transporting ATP synthase complex, coupling factor F(o)</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005634 nucleus</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0043231 intracellular membrane-bounded organelle</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0045261 proton-transporting ATP synthase complex, catalytic core F(1)</t>
+    <t xml:space="preserve">GO:0005623 cell </t>
   </si>
   <si>
     <t xml:space="preserve">GO:0005794 Golgi apparatus</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005623 cell </t>
+    <t xml:space="preserve">GO:0022627 cytosolic small ribosomal subunit</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0005793 endoplasmic reticulum-Golgi intermediate compartment</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0022627 cytosolic small ribosomal subunit</t>
+    <t xml:space="preserve">GO:0005829 cytosol</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0005783 endoplasmic reticulum</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005829 cytosol</t>
+    <t xml:space="preserve">GO:0005840 ribosome</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0005739 mitochondrion </t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005840 ribosome</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0009522 photosystem I</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0015935 small ribosomal subunit</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0016020 membrane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009536 plastid </t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0030126 COPI vesicle coat</t>
   </si>
   <si>
@@ -586,6 +608,9 @@
   </si>
   <si>
     <t xml:space="preserve">GO:0031361 integral component of thylakoid membrane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Membrane:cytoplasm</t>
   </si>
 </sst>
 </file>
@@ -849,10 +874,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="G47"/>
+      <selection pane="topLeft" activeCell="I35" activeCellId="0" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1593,10 +1618,342 @@
         <v>9</v>
       </c>
     </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I51" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(J43:K43)</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.21"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>127</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <f aca="false">SUM(B3:E3)</f>
+        <v>500</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">B3/B4</f>
+        <v>2.6</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">C3/C4</f>
+        <v>1.7887323943662</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">D3/D4</f>
+        <v>2.36170212765957</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">E3/E4</f>
+        <v>2.45762711864407</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <f aca="false">SUM(B4:E4)</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">SUM(B5:E5)</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <f aca="false">SUM(B6:E6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <f aca="false">SUM(B7:E7)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <f aca="false">SUM(B8:E8)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <f aca="false">SUM(B9:E9)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <f aca="false">SUM(B10:E10)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J12" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J13" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J14" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J15" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J16" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J17" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J18" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J19" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J20" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J21" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J22" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J23" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J24" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J25" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J26" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1609,10 +1966,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H49" activeCellId="0" sqref="H49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H48" activeCellId="0" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2301,6 +2658,13 @@
       <c r="F41" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="H41" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <f aca="false">A41+A48</f>
+        <v>127</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -2312,6 +2676,13 @@
       <c r="C42" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="H42" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <f aca="false">A42+A49</f>
+        <v>71</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -2326,6 +2697,13 @@
       <c r="D43" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="H43" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <f aca="false">A43+A50</f>
+        <v>21</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -2337,6 +2715,13 @@
       <c r="C44" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="H44" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <f aca="false">A45</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
@@ -2356,12 +2741,22 @@
       </c>
       <c r="F45" s="0" t="s">
         <v>71</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>63</v>
       </c>
+      <c r="H46" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <f aca="false">A51</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
@@ -2372,6 +2767,13 @@
       </c>
       <c r="C47" s="0" t="s">
         <v>4</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <f aca="false">A52</f>
+        <v>12</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2392,6 +2794,14 @@
       </c>
       <c r="F48" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="H48" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(B44:F44)</f>
+        <v>GO:0045261proton-transporting ATP synthase complex, catalytic core F(1)</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <f aca="false">A44</f>
+        <v>3</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,10 +2873,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2644,7 +3054,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D11,E11,F11,G11,H11)</f>
@@ -2803,6 +3213,13 @@
       <c r="F22" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="H22" s="0" t="n">
+        <f aca="false">A22+A29</f>
+        <v>111</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -2814,6 +3231,13 @@
       <c r="C23" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="H23" s="0" t="n">
+        <f aca="false">A23+A30</f>
+        <v>47</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -2828,6 +3252,13 @@
       <c r="D24" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="H24" s="0" t="n">
+        <f aca="false">A24+A32</f>
+        <v>19</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -2848,6 +3279,9 @@
       <c r="F25" s="0" t="s">
         <v>74</v>
       </c>
+      <c r="I25" s="0" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -2858,12 +3292,26 @@
       </c>
       <c r="C26" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">A25</f>
+        <v>1</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>63</v>
       </c>
+      <c r="H27" s="0" t="n">
+        <f aca="false">A31</f>
+        <v>21</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -2874,6 +3322,13 @@
       </c>
       <c r="C28" s="0" t="s">
         <v>4</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <f aca="false">A26+A33</f>
+        <v>13</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2894,6 +3349,9 @@
       </c>
       <c r="F29" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2965,10 +3423,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2987,7 +3445,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3090,7 +3548,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D8,E8,F8,G8,H8)</f>
@@ -3232,14 +3690,14 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D16,E16,F16,G16,H16)</f>
         <v>plastid</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3282,6 +3740,13 @@
       <c r="F21" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="H21" s="0" t="n">
+        <f aca="false">A21+A27</f>
+        <v>145</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -3293,6 +3758,13 @@
       <c r="C22" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="H22" s="0" t="n">
+        <f aca="false">A22+A28</f>
+        <v>59</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -3307,6 +3779,13 @@
       <c r="D23" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="H23" s="0" t="n">
+        <f aca="false">A23+A29</f>
+        <v>30</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -3317,12 +3796,25 @@
       </c>
       <c r="C24" s="0" t="s">
         <v>34</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>63</v>
       </c>
+      <c r="H25" s="0" t="n">
+        <f aca="false">A31</f>
+        <v>12</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -3333,6 +3825,13 @@
       </c>
       <c r="C26" s="0" t="s">
         <v>4</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">A30</f>
+        <v>18</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3354,6 +3853,9 @@
       <c r="F27" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="I27" s="0" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -3365,6 +3867,13 @@
       <c r="C28" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="H28" s="0" t="n">
+        <f aca="false">A24</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -3402,7 +3911,7 @@
         <v>12</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>73</v>
@@ -3511,7 +4020,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3660,13 +4169,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3674,16 +4183,16 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3691,19 +4200,19 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3711,7 +4220,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -3734,19 +4243,19 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>71</v>
@@ -3757,13 +4266,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>90</v>
@@ -3788,13 +4297,13 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>71</v>
@@ -3805,7 +4314,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>58</v>
@@ -3979,7 +4488,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>15</v>
@@ -4012,19 +4521,19 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>71</v>
@@ -4035,10 +4544,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4046,10 +4555,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4229,19 +4738,19 @@
         <v>2</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="G33" s="0" t="s">
         <v>71</v>
@@ -4272,13 +4781,13 @@
         <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>71</v>
@@ -4289,7 +4798,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>58</v>
@@ -4303,7 +4812,7 @@
         <v>1</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -4454,7 +4963,7 @@
         <v>3</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>6</v>
@@ -4488,19 +4997,19 @@
         <v>2</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="G50" s="0" t="s">
         <v>71</v>
@@ -4522,13 +5031,13 @@
         <v>1</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>71</v>
@@ -4539,13 +5048,13 @@
         <v>1</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4553,10 +5062,10 @@
         <v>1</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>7</v>
@@ -4576,19 +5085,19 @@
         <v>1</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="G55" s="0" t="s">
         <v>71</v>
@@ -4599,7 +5108,7 @@
         <v>1</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>58</v>
@@ -4633,7 +5142,7 @@
         <v>1</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>12</v>
@@ -4673,7 +5182,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4811,7 +5320,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>58</v>
@@ -4836,7 +5345,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>12</v>
@@ -4876,7 +5385,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4891,7 +5400,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4971,7 +5480,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>79</v>
@@ -4988,7 +5497,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>73</v>
@@ -5061,16 +5570,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -5089,10 +5598,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S52"/>
+  <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P29" activeCellId="0" sqref="P29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P18" activeCellId="0" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5105,6 +5614,9 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="T1" s="0" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -5123,37 +5635,49 @@
         <v>325</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>153</v>
+        <v>163</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5177,7 +5701,7 @@
         <v>92</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>154</v>
+        <v>93</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>39</v>
@@ -5192,7 +5716,7 @@
         <v>24</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="P3" s="0" t="n">
         <f aca="false">J6+J14+J18+J19</f>
@@ -5210,6 +5734,21 @@
         <f aca="false">M6+M14+M18+M19</f>
         <v>7</v>
       </c>
+      <c r="T3" s="0" t="n">
+        <f aca="false">P5/P17</f>
+        <v>10.25</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <f aca="false">Q5/Q17</f>
+        <v>0.176470588235294</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <f aca="false">R5/R17</f>
+        <v>14</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -5232,7 +5771,7 @@
         <v>76</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>30</v>
@@ -5247,7 +5786,7 @@
         <v>22</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="P4" s="0" t="n">
         <f aca="false">J4+J5+J29+J32</f>
@@ -5287,7 +5826,7 @@
         <v>34</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>14</v>
@@ -5302,7 +5841,7 @@
         <v>8</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>154</v>
+        <v>93</v>
       </c>
       <c r="P5" s="0" t="n">
         <f aca="false">J3+J15</f>
@@ -5342,7 +5881,7 @@
         <v>17</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>5</v>
@@ -5357,19 +5896,19 @@
         <v>5</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="P6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Q6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="S6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5390,7 +5929,7 @@
         <v>14</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>2</v>
@@ -5404,23 +5943,19 @@
       <c r="M7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O7" s="3" t="s">
-        <v>160</v>
+      <c r="O7" s="0" t="s">
+        <v>169</v>
       </c>
       <c r="P7" s="0" t="n">
-        <f aca="false">J34+J9</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="0" t="n">
-        <f aca="false">K34+K9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R7" s="0" t="n">
-        <f aca="false">L34+L9</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S7" s="0" t="n">
-        <f aca="false">M34+M9</f>
         <v>0</v>
       </c>
     </row>
@@ -5436,7 +5971,7 @@
         <v>13</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -5450,23 +5985,23 @@
       <c r="M8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O8" s="0" t="s">
-        <v>162</v>
+      <c r="O8" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="P8" s="0" t="n">
-        <f aca="false">J33+J8</f>
-        <v>1</v>
+        <f aca="false">J34+J9</f>
+        <v>2</v>
       </c>
       <c r="Q8" s="0" t="n">
-        <f aca="false">K33+K8</f>
-        <v>13</v>
+        <f aca="false">K34+K9</f>
+        <v>2</v>
       </c>
       <c r="R8" s="0" t="n">
-        <f aca="false">L33+L8</f>
-        <v>0</v>
+        <f aca="false">L34+L9</f>
+        <v>3</v>
       </c>
       <c r="S8" s="0" t="n">
-        <f aca="false">M33+M8</f>
+        <f aca="false">M34+M9</f>
         <v>0</v>
       </c>
     </row>
@@ -5488,7 +6023,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>163</v>
+        <v>101</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>1</v>
@@ -5502,23 +6037,23 @@
       <c r="M9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O9" s="3" t="s">
-        <v>164</v>
+      <c r="O9" s="0" t="s">
+        <v>172</v>
       </c>
       <c r="P9" s="0" t="n">
-        <f aca="false">J20+J27</f>
-        <v>2</v>
+        <f aca="false">J33+J8</f>
+        <v>1</v>
       </c>
       <c r="Q9" s="0" t="n">
-        <f aca="false">K20+K27</f>
-        <v>0</v>
+        <f aca="false">K33+K8</f>
+        <v>13</v>
       </c>
       <c r="R9" s="0" t="n">
-        <f aca="false">L20+L27</f>
+        <f aca="false">L33+L8</f>
         <v>0</v>
       </c>
       <c r="S9" s="0" t="n">
-        <f aca="false">M20+M27</f>
+        <f aca="false">M33+M8</f>
         <v>0</v>
       </c>
     </row>
@@ -5534,7 +6069,7 @@
         <v>5</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -5548,19 +6083,23 @@
       <c r="M10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O10" s="0" t="s">
-        <v>166</v>
+      <c r="O10" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="P10" s="0" t="n">
-        <v>1</v>
+        <f aca="false">J20+J27</f>
+        <v>2</v>
       </c>
       <c r="Q10" s="0" t="n">
+        <f aca="false">K20+K27</f>
         <v>0</v>
       </c>
       <c r="R10" s="0" t="n">
+        <f aca="false">L20+L27</f>
         <v>0</v>
       </c>
       <c r="S10" s="0" t="n">
+        <f aca="false">M20+M27</f>
         <v>0</v>
       </c>
     </row>
@@ -5579,7 +6118,7 @@
         <v>5</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>4</v>
@@ -5593,23 +6132,19 @@
       <c r="M11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O11" s="3" t="s">
-        <v>168</v>
+      <c r="O11" s="0" t="s">
+        <v>176</v>
       </c>
       <c r="P11" s="0" t="n">
-        <f aca="false">J17+J25</f>
         <v>1</v>
       </c>
       <c r="Q11" s="0" t="n">
-        <f aca="false">K17+K25</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R11" s="0" t="n">
-        <f aca="false">L17+L25</f>
         <v>0</v>
       </c>
       <c r="S11" s="0" t="n">
-        <f aca="false">M17+M25</f>
         <v>0</v>
       </c>
     </row>
@@ -5628,7 +6163,7 @@
         <v>4</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>2</v>
@@ -5643,22 +6178,22 @@
         <v>0</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="P12" s="0" t="n">
-        <f aca="false">J21+J22+J23+J24</f>
+        <f aca="false">J17+J25</f>
         <v>1</v>
       </c>
       <c r="Q12" s="0" t="n">
-        <f aca="false">K21+K22+K23+K24</f>
-        <v>3</v>
+        <f aca="false">K17+K25</f>
+        <v>2</v>
       </c>
       <c r="R12" s="0" t="n">
-        <f aca="false">L21+L22+L23+L24</f>
+        <f aca="false">L17+L25</f>
         <v>0</v>
       </c>
       <c r="S12" s="0" t="n">
-        <f aca="false">M21+M22+M23+M24</f>
+        <f aca="false">M17+M25</f>
         <v>0</v>
       </c>
     </row>
@@ -5677,7 +6212,7 @@
         <v>4</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>1</v>
@@ -5691,19 +6226,23 @@
       <c r="M13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O13" s="0" t="s">
-        <v>171</v>
+      <c r="O13" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="P13" s="0" t="n">
+        <f aca="false">J21+J22+J23+J24</f>
         <v>1</v>
       </c>
       <c r="Q13" s="0" t="n">
+        <f aca="false">K21+K22+K23+K24</f>
         <v>3</v>
       </c>
       <c r="R13" s="0" t="n">
+        <f aca="false">L21+L22+L23+L24</f>
         <v>0</v>
       </c>
       <c r="S13" s="0" t="n">
+        <f aca="false">M21+M22+M23+M24</f>
         <v>0</v>
       </c>
     </row>
@@ -5725,7 +6264,7 @@
         <v>4</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>2</v>
@@ -5739,23 +6278,19 @@
       <c r="M14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>173</v>
+      <c r="O14" s="0" t="s">
+        <v>179</v>
       </c>
       <c r="P14" s="0" t="n">
-        <f aca="false">J16+J11</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="0" t="n">
-        <f aca="false">K16+K11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R14" s="0" t="n">
-        <f aca="false">L16+L11</f>
         <v>0</v>
       </c>
       <c r="S14" s="0" t="n">
-        <f aca="false">M16+M11</f>
         <v>0</v>
       </c>
     </row>
@@ -5774,7 +6309,7 @@
         <v>4</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>174</v>
+        <v>99</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>2</v>
@@ -5788,20 +6323,24 @@
       <c r="M15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O15" s="0" t="s">
-        <v>175</v>
+      <c r="O15" s="3" t="s">
+        <v>182</v>
       </c>
       <c r="P15" s="0" t="n">
-        <v>0</v>
+        <f aca="false">J16+J11</f>
+        <v>6</v>
       </c>
       <c r="Q15" s="0" t="n">
-        <v>0</v>
+        <f aca="false">K16+K11</f>
+        <v>2</v>
       </c>
       <c r="R15" s="0" t="n">
+        <f aca="false">L16+L11</f>
         <v>0</v>
       </c>
       <c r="S15" s="0" t="n">
-        <v>1</v>
+        <f aca="false">M16+M11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5819,7 +6358,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>2</v>
@@ -5834,7 +6373,7 @@
         <v>0</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="P16" s="0" t="n">
         <v>1</v>
@@ -5861,7 +6400,7 @@
         <v>2</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>0</v>
@@ -5876,7 +6415,7 @@
         <v>0</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">J10+J12+J7</f>
@@ -5910,7 +6449,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>1</v>
@@ -5927,7 +6466,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1</v>
@@ -5940,7 +6479,7 @@
         <v>2</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>0</v>
@@ -5967,7 +6506,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>1</v>
@@ -5994,7 +6533,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>0</v>
@@ -6021,7 +6560,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>1</v>
@@ -6048,7 +6587,7 @@
         <v>1</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="J23" s="0" t="n">
         <v>0</v>
@@ -6075,7 +6614,7 @@
         <v>1</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>0</v>
@@ -6102,7 +6641,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>1</v>
@@ -6129,7 +6668,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>1</v>
@@ -6156,7 +6695,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>1</v>
@@ -6183,7 +6722,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="J28" s="0" t="n">
         <v>0</v>
@@ -6210,7 +6749,7 @@
         <v>1</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>1</v>
@@ -6227,7 +6766,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>1</v>
@@ -6237,7 +6776,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>0</v>
@@ -6264,7 +6803,7 @@
         <v>1</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="J31" s="0" t="n">
         <v>1</v>
@@ -6291,7 +6830,7 @@
         <v>1</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="J32" s="0" t="n">
         <v>1</v>
@@ -6318,7 +6857,7 @@
         <v>1</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>1</v>
@@ -6345,7 +6884,7 @@
         <v>1</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
made nb to sort unipept lca ouput
</commit_message>
<xml_diff>
--- a/analyses/unipept/GO-terms/GO-summary.xlsx
+++ b/analyses/unipept/GO-terms/GO-summary.xlsx
@@ -1712,41 +1712,41 @@
         <v>500</v>
       </c>
       <c r="G3" s="0" t="n">
-        <f aca="false">B3/B4</f>
+        <f aca="false">B3/B10</f>
         <v>2.6</v>
       </c>
       <c r="H3" s="0" t="n">
-        <f aca="false">C3/C4</f>
+        <f aca="false">C3/C10</f>
         <v>1.7887323943662</v>
       </c>
       <c r="I3" s="0" t="n">
-        <f aca="false">D3/D4</f>
+        <f aca="false">D3/D10</f>
         <v>2.36170212765957</v>
       </c>
       <c r="J3" s="0" t="n">
-        <f aca="false">E3/E4</f>
+        <f aca="false">E3/E10</f>
         <v>2.45762711864407</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">SUM(B4:E4)</f>
-        <v>222</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,23 +1772,23 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="0" t="n">
         <f aca="false">SUM(B6:E6)</f>
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1814,65 +1814,65 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">SUM(B8:E8)</f>
-        <v>65</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">SUM(B9:E9)</f>
-        <v>37</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">SUM(B10:E10)</f>
-        <v>4</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5601,7 +5601,7 @@
   <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P18" activeCellId="0" sqref="P18"/>
+      <selection pane="topLeft" activeCell="P22" activeCellId="0" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>